<commit_message>
Edit and save File
</commit_message>
<xml_diff>
--- a/src/dataEngine/DataEngine.xlsx
+++ b/src/dataEngine/DataEngine.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="TestSuite" sheetId="2" r:id="rId1"/>
@@ -1745,8 +1745,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2180,8 +2180,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>